<commit_message>
Now it is working with different path but the texts that included are seperately in the file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,36 +448,1136 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>file01.txt</t>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dfsdfs</t>
+          <t>Who would’ve thought their bond would grow this strong? 🥹💕</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>file02.txt</t>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>file03.txt</t>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dsafsdfdsa</t>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>🐻‍❄️LIKE | SAVE | SHARE🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Follow @babybearyuki for your daily dose of hugs &amp; smiles! </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram#dogmodel#doggo#doglovers#dogstagram#instadog#samoyed#puppiesofinstagram#samoyedsofinstagram#puppy#animalsofinstagram#aussiesofinstagram#funny#doggie#happydog#funnydog#fluffydog#dogslife#pet#犬のいる生活#dogstagram#samoyedpage#hugs#bestwoof#dogood#dogmom#doglife#dogofinsta#cutedoggy#barked</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2022-09-14_13-43-42_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Polar opposites attract am I right? 🐻💕🐻‍❄️</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>🐻‍❄️LIKE | SAVE | SHARE🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Follow @babybearyuki for your daily dose of hugs &amp; smiles! </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram#dogmodel#doggo#doglovers#dogstagram#instadog#samoyed#puppiesofinstagram#samoyedsofinstagram#puppy#animalsofinstagram#aussiesofinstagram#funny#doggie#happydog#funnydog#fluffydog#dogslife#pet#犬のいる生活#dogstagram#samoyedpage#hugs#bestwoof#dogood#dogmom#doglife#dogofinsta#cutedoggy#barked</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2022-09-17_13-36-24_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Trying the ✨Painters Tape Challenge✨! Who did it better? 🐻 or 🐻‍❄️?</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo: @halfhuskybros </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>🐻‍❄️LIKE | SAVE | SHARE🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Follow @babybearyuki for your daily dose of hugs &amp; smiles! </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram#dogmodel#doggo#doglovers#dogstagram#instadog#samoyed#puppiesofinstagram#samoyedsofinstagram#puppy#animalsofinstagram#aussiesofinstagram#funny#doggie#happydog#funnydog#fluffydog#dogslife#pet#犬のいる生活#dogstagram#samoyedpage#hugs#bestwoof#dogood#dogmom#doglife#dogofinsta#cutedoggy#barked</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2022-09-18_13-38-26_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>That’s my ✨ PUPPY DOG ✨ 🐻‍❄️💕🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>🐻‍❄️LIKE | SAVE | SHARE🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Follow @babybearyuki for your daily dose of hugs &amp; smiles! </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram#dogmodel#doggo#doglovers#dogstagram#instadog#samoyed#puppiesofinstagram#samoyedsofinstagram#puppy#animalsofinstagram#aussiesofinstagram#funny#doggie#happydog#funnydog#fluffydog#dogslife#pet#犬のいる生活#dogstagram#samoyedpage#hugs#bestwoof#dogood#dogmom#doglife#dogofinsta#cutedoggy#barked</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2022-09-25_13-53-02_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>✨VIRTUAL HUGS✨ just for you! 💌</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐻‍❄️LIKE | SAVE | SHARE🐻 </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Follow @babybearyuki for your daily dose of hugs &amp; smiles! </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">. </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">. </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌◌</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram #doglovers #dog #samoyed #australianshepherd #samoyedsofinstagram #puppy #weeklyfluff #animalsofinstagram #aussiesofinstagram #happydog #goldenretriever #fluffydog #pet #犬のいる生活 #doghug #bestwoof #cute #barked</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-01-07_17-43-03_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Yuki‘s favorite ✨PUPPY DOG✨🐻‍❄️💕🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>FOLLOW &amp; SHARE @babybearyuki for more hugs &amp; smiles!</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>🐻‍❄️💕🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram #weeklyfluff #australianshepherd #samoyed #dog #cuteanimals #puppy</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2023-07-25_17-32-17_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>A hug a day, keeps all worries away! 💕</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FOLLOW &amp; SHARE @babybearyuki for more hugs &amp; smiles!</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>🐻‍❄️💕🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram #weeklyfluff #australianshepherd #samoyed #dog #cuteanimals #puppy</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2023-07-29_16-44-01_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Just cuteness, no brains 🥰</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>FOLLOW &amp; SHARE @babybearyuki for more hugs &amp; smiles!</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>🐻‍❄️💕🐻</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>#dogsofinstagram #weeklyfluff #australianshepherd #samoyed #dog #cuteanimals #puppy</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2023-08-29_17-55-29_UTC.txt</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Credit: babybearyuki</t>
         </is>
       </c>
     </row>

</xml_diff>